<commit_message>
Flipkart application new Repo
</commit_message>
<xml_diff>
--- a/src/main/java/nandha/resources/testdata.xlsx
+++ b/src/main/java/nandha/resources/testdata.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnand\NK\Flipkart\SeleniumFramework\src\main\java\nandha\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36347F61-E01D-4A2B-AED6-50274C251213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13592615-CFB9-4991-B3E0-9CA036FBA388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
   <si>
     <t>searchdata</t>
   </si>
@@ -109,12 +109,65 @@
   </si>
   <si>
     <t>30% or more</t>
+  </si>
+  <si>
+    <t>Mobiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pincode</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Delivery Date</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Sort</t>
+  </si>
+  <si>
+    <t>Relevance</t>
+  </si>
+  <si>
+    <t>Popularity</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy M34 5G without charger (Prism Silver, 128 GB)</t>
+  </si>
+  <si>
+    <t>24 Jul, Wednesday</t>
+  </si>
+  <si>
+    <t>Highlights
+6 GB RAM | 128 GB ROM
+16.51 cm (6.5 inch) Display
+50MP Rear Camera
+6000 mAh Battery</t>
+  </si>
+  <si>
+    <t>₹15,495</t>
+  </si>
+  <si>
+    <t>SAMSUNG Galaxy M34 5G (Waterfall Blue, 128 GB)</t>
+  </si>
+  <si>
+    <t>25 Jul, Thursday</t>
+  </si>
+  <si>
+    <t>₹15,399</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,35 +499,35 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.44140625"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.44140625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>4</v>
       </c>
     </row>
@@ -485,113 +538,152 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.109375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.109375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.88671875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.0"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.109375"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="18.6640625"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.44140625"/>
+    <col min="8" max="8" customWidth="true" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H1" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="0">
+        <v>15000</v>
+      </c>
+      <c r="D2" s="0">
+        <v>30000</v>
+      </c>
+      <c r="E2" s="0">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="I2" s="0">
+        <v>636903</v>
+      </c>
+      <c r="J2" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="K2" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="L2" t="s" s="0">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="C3" s="0">
+        <v>15000</v>
+      </c>
+      <c r="D3" s="0">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="0">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0">
         <v>10000</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="D4" s="0">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="0">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s" s="0">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>15000</v>
-      </c>
-      <c r="D3">
-        <v>20000</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4">
-        <v>10000</v>
-      </c>
-      <c r="D4">
-        <v>20000</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10" t="s" s="0">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -610,44 +702,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="11.21875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>13</v>
       </c>
     </row>
@@ -666,14 +758,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="26.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>3</v>
       </c>
     </row>
@@ -681,7 +773,7 @@
       <c r="A2" s="1">
         <v>9452271671</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>4</v>
       </c>
     </row>

</xml_diff>